<commit_message>
Chuyển lưu trữ điểm sang Google Sheet API
</commit_message>
<xml_diff>
--- a/data/questions.xlsx
+++ b/data/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danghuuphuoc/Documents/Tai Lieu Day/quiz-node/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29540171-CC28-9341-86FB-033EB439E26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29588AC3-ACF5-2242-B8B9-1FCCE7D2D5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="6000" windowWidth="25080" windowHeight="17440" xr2:uid="{C9331AA8-6F23-D44E-A801-05F4E988B16F}"/>
+    <workbookView xWindow="32280" yWindow="580" windowWidth="17260" windowHeight="17440" xr2:uid="{C9331AA8-6F23-D44E-A801-05F4E988B16F}"/>
   </bookViews>
   <sheets>
     <sheet name="DSCau" sheetId="1" r:id="rId1"/>
@@ -2547,7 +2547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404D1119-1C3A-E547-9278-4B9B5898D530}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
cập nhật nội dung câu hỏi
</commit_message>
<xml_diff>
--- a/data/questions.xlsx
+++ b/data/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danghuuphuoc/Documents/Tai Lieu Day/quiz-node/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29588AC3-ACF5-2242-B8B9-1FCCE7D2D5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C97A3C-5D39-6E4F-A9E1-8D5881C6497B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32280" yWindow="580" windowWidth="17260" windowHeight="17440" xr2:uid="{C9331AA8-6F23-D44E-A801-05F4E988B16F}"/>
+    <workbookView xWindow="20240" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{C9331AA8-6F23-D44E-A801-05F4E988B16F}"/>
   </bookViews>
   <sheets>
     <sheet name="DSCau" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="690">
   <si>
     <t>ID</t>
   </si>
@@ -2117,6 +2117,39 @@
   </si>
   <si>
     <t>7.10</t>
+  </si>
+  <si>
+    <t>A2.11</t>
+  </si>
+  <si>
+    <t>A2.12</t>
+  </si>
+  <si>
+    <t>Máy chiếu</t>
+  </si>
+  <si>
+    <t>Máy quét (scanner)</t>
+  </si>
+  <si>
+    <t>Bạn An Bình cần quét tài liệu giấy để lưu trữ trên máy tính. Thiết bị ngoại vi nào phù hợp nhất cho công việc này?</t>
+  </si>
+  <si>
+    <t>A2.13</t>
+  </si>
+  <si>
+    <t>A2.14</t>
+  </si>
+  <si>
+    <t>Webcam</t>
+  </si>
+  <si>
+    <t>Bạn Thiên Thiên muốn trình chiếu nội dung từ máy tính cá nhân lên màn hình lớn. Thiết bị ngoại vi nào cần được kết nối?</t>
+  </si>
+  <si>
+    <t>Nguyễn Nhi muốn gọi video chất lượng cao từ máy tính cá nhân, bạn cần kết nối thiết bị ngoại vi nào sau đây?</t>
+  </si>
+  <si>
+    <t>Thiết bị nào có chức năng chuyển văn bản, hình ảnh thành tệp ảnh số hóa?</t>
   </si>
 </sst>
 </file>
@@ -2178,7 +2211,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2203,6 +2236,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2216,7 +2255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2231,6 +2270,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2545,10 +2585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{404D1119-1C3A-E547-9278-4B9B5898D530}">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -2556,7 +2596,7 @@
     <col min="1" max="1" width="7.140625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" customWidth="1"/>
+    <col min="4" max="4" width="51" customWidth="1"/>
     <col min="5" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" customWidth="1"/>
   </cols>
@@ -3183,180 +3223,177 @@
       <c r="J21">
         <v>1</v>
       </c>
-      <c r="L21" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J22" s="5">
-        <v>1</v>
+      <c r="A22" s="14" t="s">
+        <v>679</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>686</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J22" s="14">
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>114</v>
+      <c r="A23" s="14" t="s">
+        <v>680</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>687</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>138</v>
+        <v>15</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>142</v>
+        <v>681</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>143</v>
+        <v>682</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>144</v>
+        <v>686</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J23">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="J23" s="14">
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>115</v>
+      <c r="A24" s="14" t="s">
+        <v>684</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>688</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>145</v>
+        <v>15</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>146</v>
+        <v>681</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>147</v>
+        <v>682</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>148</v>
+        <v>686</v>
       </c>
       <c r="I24" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J24">
-        <v>1</v>
+      <c r="J24" s="14">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>116</v>
+      <c r="A25" s="14" t="s">
+        <v>685</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>689</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>174</v>
+        <v>15</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>149</v>
+        <v>681</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>150</v>
+        <v>682</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>151</v>
+        <v>686</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="J25">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="J25" s="14">
+        <v>2</v>
+      </c>
+      <c r="L25" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="I26" s="9" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="I26" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>130</v>
+      <c r="A27" t="s">
+        <v>126</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>113</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="I27" s="9" t="s">
         <v>7</v>
@@ -3366,26 +3403,26 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>131</v>
+      <c r="A28" t="s">
+        <v>127</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>113</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>7</v>
@@ -3395,55 +3432,58 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>132</v>
+      <c r="A29" t="s">
+        <v>128</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>113</v>
       </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
       <c r="D29" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="J29">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>133</v>
+      <c r="A30" t="s">
+        <v>129</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>113</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="I30" s="9" t="s">
         <v>7</v>
@@ -3453,128 +3493,244 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>134</v>
+      <c r="A31" t="s">
+        <v>130</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>113</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J31">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>135</v>
+      <c r="A32" t="s">
+        <v>131</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>113</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J32">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>136</v>
+      <c r="A33" t="s">
+        <v>132</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>113</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="I33" s="9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J33">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>137</v>
+      <c r="A34" t="s">
+        <v>133</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>136</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D38" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E38" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G38" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="H38" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="I34" s="9" t="s">
+      <c r="I38" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="J34">
+      <c r="J38">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5 C8 C25 C34" xr:uid="{8D0A2AEC-5FF2-A04E-8E8C-7C944DEF2AB0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5 C8 C29 C38" xr:uid="{8D0A2AEC-5FF2-A04E-8E8C-7C944DEF2AB0}">
       <formula1>"multiple"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3587,7 +3743,7 @@
           <x14:formula1>
             <xm:f>ChuDe!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B34</xm:sqref>
+          <xm:sqref>B2:B38</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9050C982-4DD8-AC44-A5C3-700A3EEC787B}">
           <x14:formula1>
@@ -3677,7 +3833,7 @@
         <v>109</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -3705,7 +3861,7 @@
         <v>113</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>1</v>

</xml_diff>